<commit_message>
work in progress adding to control
</commit_message>
<xml_diff>
--- a/Project_B/control_signals_template.xlsx
+++ b/Project_B/control_signals_template.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="85">
   <si>
     <t>Instruction</t>
   </si>
@@ -60,6 +60,9 @@
     <t>Shift</t>
   </si>
   <si>
+    <t>UpperImm</t>
+  </si>
+  <si>
     <t>addi</t>
   </si>
   <si>
@@ -70,14 +73,15 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <color rgb="FF000000"/>
+      </rPr>
       <t xml:space="preserve">0 </t>
     </r>
     <r>
       <rPr>
-        <rFont val="Calibri"/>
         <i/>
-        <color theme="1"/>
-        <sz val="12.0"/>
+        <color rgb="FF000000"/>
       </rPr>
       <t>[addi uses rt as destination register rather than rd]</t>
     </r>
@@ -337,7 +341,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -348,6 +352,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
@@ -646,7 +653,9 @@
       <c r="N2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="2"/>
+      <c r="O2" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
@@ -661,16 +670,16 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="B3" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="C3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="2" t="s">
         <v>17</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="E3" s="2">
         <v>0.0</v>
@@ -679,30 +688,32 @@
         <v>0.0</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J3" s="2">
         <v>0.0</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N3" s="3">
         <v>0.0</v>
       </c>
-      <c r="O3" s="2"/>
+      <c r="O3" s="3">
+        <v>0.0</v>
+      </c>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
@@ -717,13 +728,13 @@
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D4" s="2">
         <v>1.0</v>
@@ -741,7 +752,7 @@
         <v>0.0</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J4" s="2">
         <v>0.0</v>
@@ -758,7 +769,9 @@
       <c r="N4" s="3">
         <v>0.0</v>
       </c>
-      <c r="O4" s="2"/>
+      <c r="O4" s="3">
+        <v>0.0</v>
+      </c>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
@@ -773,13 +786,13 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="B5" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="C5" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5" s="2">
         <v>0.0</v>
@@ -797,7 +810,7 @@
         <v>0.0</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J5" s="2">
         <v>0.0</v>
@@ -814,7 +827,9 @@
       <c r="N5" s="3">
         <v>0.0</v>
       </c>
-      <c r="O5" s="2"/>
+      <c r="O5" s="3">
+        <v>0.0</v>
+      </c>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
@@ -829,13 +844,13 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D6" s="2">
         <v>1.0</v>
@@ -853,7 +868,7 @@
         <v>0.0</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J6" s="2">
         <v>0.0</v>
@@ -870,7 +885,9 @@
       <c r="N6" s="3">
         <v>0.0</v>
       </c>
-      <c r="O6" s="2"/>
+      <c r="O6" s="3">
+        <v>0.0</v>
+      </c>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
@@ -885,13 +902,13 @@
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D7" s="2">
         <v>1.0</v>
@@ -909,7 +926,7 @@
         <v>0.0</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J7" s="2">
         <v>0.0</v>
@@ -926,7 +943,9 @@
       <c r="N7" s="3">
         <v>0.0</v>
       </c>
-      <c r="O7" s="2"/>
+      <c r="O7" s="3">
+        <v>0.0</v>
+      </c>
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
@@ -941,13 +960,13 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="B8" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="C8" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D8" s="2">
         <v>0.0</v>
@@ -965,7 +984,7 @@
         <v>0.0</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J8" s="2">
         <v>0.0</v>
@@ -982,7 +1001,9 @@
       <c r="N8" s="3">
         <v>0.0</v>
       </c>
-      <c r="O8" s="2"/>
+      <c r="O8" s="3">
+        <v>0.0</v>
+      </c>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
@@ -997,13 +1018,13 @@
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="B9" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="C9" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D9" s="2">
         <v>0.0</v>
@@ -1014,14 +1035,14 @@
       <c r="F9" s="2">
         <v>0.0</v>
       </c>
-      <c r="G9" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="H9" s="2">
-        <v>1.0</v>
+      <c r="G9" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0.0</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J9" s="2">
         <v>0.0</v>
@@ -1038,7 +1059,9 @@
       <c r="N9" s="3">
         <v>0.0</v>
       </c>
-      <c r="O9" s="2"/>
+      <c r="O9" s="3">
+        <v>1.0</v>
+      </c>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
@@ -1053,13 +1076,13 @@
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="2" t="s">
         <v>37</v>
       </c>
+      <c r="B10" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="C10" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D10" s="2">
         <v>0.0</v>
@@ -1070,31 +1093,33 @@
       <c r="F10" s="2">
         <v>0.0</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="3">
         <v>1.0</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="3">
         <v>1.0</v>
       </c>
-      <c r="I10" s="2" t="s">
-        <v>20</v>
+      <c r="I10" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="J10" s="2">
         <v>0.0</v>
       </c>
-      <c r="K10" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="L10" s="2">
+      <c r="K10" s="3">
         <v>1.0</v>
       </c>
-      <c r="M10" s="2">
+      <c r="L10" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="M10" s="3">
         <v>1.0</v>
       </c>
       <c r="N10" s="3">
         <v>0.0</v>
       </c>
-      <c r="O10" s="2"/>
+      <c r="O10" s="3">
+        <v>0.0</v>
+      </c>
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
@@ -1109,13 +1134,13 @@
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D11" s="2">
         <v>1.0</v>
@@ -1133,7 +1158,7 @@
         <v>0.0</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J11" s="2">
         <v>0.0</v>
@@ -1150,7 +1175,9 @@
       <c r="N11" s="3">
         <v>0.0</v>
       </c>
-      <c r="O11" s="2"/>
+      <c r="O11" s="3">
+        <v>0.0</v>
+      </c>
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
@@ -1165,13 +1192,13 @@
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D12" s="2">
         <v>1.0</v>
@@ -1189,7 +1216,7 @@
         <v>0.0</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J12" s="2">
         <v>0.0</v>
@@ -1206,7 +1233,9 @@
       <c r="N12" s="3">
         <v>0.0</v>
       </c>
-      <c r="O12" s="2"/>
+      <c r="O12" s="3">
+        <v>0.0</v>
+      </c>
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
@@ -1221,13 +1250,13 @@
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" s="2" t="s">
         <v>45</v>
       </c>
+      <c r="B13" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="C13" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D13" s="2">
         <v>0.0</v>
@@ -1245,7 +1274,7 @@
         <v>0.0</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J13" s="2">
         <v>0.0</v>
@@ -1262,7 +1291,9 @@
       <c r="N13" s="3">
         <v>0.0</v>
       </c>
-      <c r="O13" s="2"/>
+      <c r="O13" s="3">
+        <v>0.0</v>
+      </c>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
@@ -1277,13 +1308,13 @@
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D14" s="2">
         <v>1.0</v>
@@ -1301,7 +1332,7 @@
         <v>0.0</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J14" s="2">
         <v>0.0</v>
@@ -1318,7 +1349,9 @@
       <c r="N14" s="3">
         <v>0.0</v>
       </c>
-      <c r="O14" s="2"/>
+      <c r="O14" s="3">
+        <v>0.0</v>
+      </c>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
@@ -1333,13 +1366,13 @@
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" s="2" t="s">
         <v>50</v>
       </c>
+      <c r="B15" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="C15" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D15" s="2">
         <v>0.0</v>
@@ -1357,7 +1390,7 @@
         <v>0.0</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J15" s="2">
         <v>0.0</v>
@@ -1374,7 +1407,9 @@
       <c r="N15" s="3">
         <v>0.0</v>
       </c>
-      <c r="O15" s="2"/>
+      <c r="O15" s="3">
+        <v>0.0</v>
+      </c>
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
@@ -1389,13 +1424,13 @@
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D16" s="2">
         <v>1.0</v>
@@ -1413,7 +1448,7 @@
         <v>0.0</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J16" s="2">
         <v>0.0</v>
@@ -1430,7 +1465,9 @@
       <c r="N16" s="3">
         <v>0.0</v>
       </c>
-      <c r="O16" s="2"/>
+      <c r="O16" s="3">
+        <v>0.0</v>
+      </c>
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
@@ -1445,13 +1482,13 @@
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B17" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="B17" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="C17" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D17" s="2">
         <v>0.0</v>
@@ -1469,7 +1506,7 @@
         <v>0.0</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J17" s="2">
         <v>0.0</v>
@@ -1486,7 +1523,9 @@
       <c r="N17" s="3">
         <v>0.0</v>
       </c>
-      <c r="O17" s="2"/>
+      <c r="O17" s="3">
+        <v>0.0</v>
+      </c>
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
@@ -1501,13 +1540,13 @@
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B18" s="2" t="s">
         <v>57</v>
       </c>
+      <c r="B18" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="C18" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D18" s="2">
         <v>0.0</v>
@@ -1524,8 +1563,8 @@
       <c r="H18" s="2">
         <v>0.0</v>
       </c>
-      <c r="I18" s="4" t="s">
-        <v>53</v>
+      <c r="I18" s="5" t="s">
+        <v>54</v>
       </c>
       <c r="J18" s="2">
         <v>0.0</v>
@@ -1542,7 +1581,9 @@
       <c r="N18" s="3">
         <v>0.0</v>
       </c>
-      <c r="O18" s="2"/>
+      <c r="O18" s="3">
+        <v>0.0</v>
+      </c>
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
@@ -1557,13 +1598,13 @@
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D19" s="2">
         <v>1.0</v>
@@ -1580,8 +1621,8 @@
       <c r="H19" s="2">
         <v>0.0</v>
       </c>
-      <c r="I19" s="4" t="s">
-        <v>53</v>
+      <c r="I19" s="5" t="s">
+        <v>54</v>
       </c>
       <c r="J19" s="2">
         <v>0.0</v>
@@ -1598,7 +1639,9 @@
       <c r="N19" s="3">
         <v>0.0</v>
       </c>
-      <c r="O19" s="2"/>
+      <c r="O19" s="3">
+        <v>0.0</v>
+      </c>
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
@@ -1613,13 +1656,13 @@
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D20" s="2">
         <v>1.0</v>
@@ -1637,7 +1680,7 @@
         <v>0.0</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J20" s="2">
         <v>0.0</v>
@@ -1654,7 +1697,9 @@
       <c r="N20" s="3">
         <v>0.0</v>
       </c>
-      <c r="O20" s="2"/>
+      <c r="O20" s="3">
+        <v>0.0</v>
+      </c>
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
       <c r="R20" s="2"/>
@@ -1669,13 +1714,13 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D21" s="2">
         <v>1.0</v>
@@ -1693,7 +1738,7 @@
         <v>0.0</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J21" s="2">
         <v>0.0</v>
@@ -1710,7 +1755,9 @@
       <c r="N21" s="3">
         <v>0.0</v>
       </c>
-      <c r="O21" s="2"/>
+      <c r="O21" s="3">
+        <v>0.0</v>
+      </c>
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
       <c r="R21" s="2"/>
@@ -1725,13 +1772,13 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D22" s="2">
         <v>1.0</v>
@@ -1749,7 +1796,7 @@
         <v>0.0</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J22" s="2">
         <v>0.0</v>
@@ -1766,7 +1813,9 @@
       <c r="N22" s="3">
         <v>0.0</v>
       </c>
-      <c r="O22" s="2"/>
+      <c r="O22" s="3">
+        <v>0.0</v>
+      </c>
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
@@ -1781,13 +1830,13 @@
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>67</v>
+        <v>26</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="D23" s="2">
         <v>1.0</v>
@@ -1804,8 +1853,8 @@
       <c r="H23" s="2">
         <v>0.0</v>
       </c>
-      <c r="I23" s="4" t="s">
-        <v>61</v>
+      <c r="I23" s="5" t="s">
+        <v>62</v>
       </c>
       <c r="J23" s="2">
         <v>0.0</v>
@@ -1822,7 +1871,9 @@
       <c r="N23" s="3">
         <v>1.0</v>
       </c>
-      <c r="O23" s="2"/>
+      <c r="O23" s="3">
+        <v>0.0</v>
+      </c>
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
@@ -1837,13 +1888,13 @@
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D24" s="2">
         <v>1.0</v>
@@ -1860,8 +1911,8 @@
       <c r="H24" s="2">
         <v>0.0</v>
       </c>
-      <c r="I24" s="4" t="s">
-        <v>63</v>
+      <c r="I24" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="J24" s="2">
         <v>0.0</v>
@@ -1878,7 +1929,9 @@
       <c r="N24" s="3">
         <v>1.0</v>
       </c>
-      <c r="O24" s="2"/>
+      <c r="O24" s="3">
+        <v>0.0</v>
+      </c>
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
@@ -1893,13 +1946,13 @@
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D25" s="2">
         <v>1.0</v>
@@ -1916,8 +1969,8 @@
       <c r="H25" s="2">
         <v>0.0</v>
       </c>
-      <c r="I25" s="4" t="s">
-        <v>65</v>
+      <c r="I25" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="J25" s="2">
         <v>0.0</v>
@@ -1934,7 +1987,9 @@
       <c r="N25" s="3">
         <v>1.0</v>
       </c>
-      <c r="O25" s="2"/>
+      <c r="O25" s="3">
+        <v>0.0</v>
+      </c>
       <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
@@ -1949,13 +2004,13 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>59</v>
+        <v>73</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D26" s="2">
         <v>0.0</v>
@@ -1973,7 +2028,7 @@
         <v>0.0</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J26" s="2">
         <v>1.0</v>
@@ -1990,7 +2045,9 @@
       <c r="N26" s="3">
         <v>0.0</v>
       </c>
-      <c r="O26" s="2"/>
+      <c r="O26" s="3">
+        <v>0.0</v>
+      </c>
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
       <c r="R26" s="2"/>
@@ -2005,13 +2062,13 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D27" s="2">
         <v>1.0</v>
@@ -2029,7 +2086,7 @@
         <v>0.0</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="J27" s="2">
         <v>0.0</v>
@@ -2046,7 +2103,9 @@
       <c r="N27" s="3">
         <v>0.0</v>
       </c>
-      <c r="O27" s="2"/>
+      <c r="O27" s="3">
+        <v>0.0</v>
+      </c>
       <c r="P27" s="2"/>
       <c r="Q27" s="2"/>
       <c r="R27" s="2"/>
@@ -2061,13 +2120,13 @@
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D28" s="2">
         <v>1.0</v>
@@ -2084,8 +2143,8 @@
       <c r="H28" s="2">
         <v>0.0</v>
       </c>
-      <c r="I28" s="4" t="s">
-        <v>75</v>
+      <c r="I28" s="5" t="s">
+        <v>76</v>
       </c>
       <c r="J28" s="2">
         <v>0.0</v>
@@ -2102,7 +2161,9 @@
       <c r="N28" s="3">
         <v>0.0</v>
       </c>
-      <c r="O28" s="2"/>
+      <c r="O28" s="3">
+        <v>0.0</v>
+      </c>
       <c r="P28" s="2"/>
       <c r="Q28" s="2"/>
       <c r="R28" s="2"/>
@@ -2117,13 +2178,13 @@
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D29" s="2">
         <v>0.0</v>
@@ -2154,7 +2215,9 @@
       <c r="N29" s="3">
         <v>0.0</v>
       </c>
-      <c r="O29" s="2"/>
+      <c r="O29" s="3">
+        <v>0.0</v>
+      </c>
       <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
       <c r="R29" s="2"/>
@@ -2169,13 +2232,13 @@
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D30" s="2">
         <v>0.0</v>
@@ -2206,7 +2269,9 @@
       <c r="N30" s="3">
         <v>0.0</v>
       </c>
-      <c r="O30" s="2"/>
+      <c r="O30" s="3">
+        <v>0.0</v>
+      </c>
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
       <c r="R30" s="2"/>
@@ -2221,16 +2286,16 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E31" s="2">
         <v>1.0</v>
@@ -2258,7 +2323,9 @@
       <c r="N31" s="3">
         <v>0.0</v>
       </c>
-      <c r="O31" s="2"/>
+      <c r="O31" s="3">
+        <v>0.0</v>
+      </c>
       <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
@@ -2273,13 +2340,13 @@
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D32" s="2">
         <v>1.0</v>
@@ -2310,7 +2377,9 @@
       <c r="N32" s="3">
         <v>0.0</v>
       </c>
-      <c r="O32" s="2"/>
+      <c r="O32" s="3">
+        <v>0.0</v>
+      </c>
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
@@ -2325,16 +2394,16 @@
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E33" s="2">
         <v>1.0</v>
@@ -2362,7 +2431,9 @@
       <c r="N33" s="3">
         <v>0.0</v>
       </c>
-      <c r="O33" s="2"/>
+      <c r="O33" s="3">
+        <v>0.0</v>
+      </c>
       <c r="P33" s="2"/>
       <c r="Q33" s="2"/>
       <c r="R33" s="2"/>

</xml_diff>

<commit_message>
Added Shift, Sign, and UpperImm to control and processor
</commit_message>
<xml_diff>
--- a/Project_B/control_signals_template.xlsx
+++ b/Project_B/control_signals_template.xlsx
@@ -54,10 +54,10 @@
     <t>s_RegWr</t>
   </si>
   <si>
-    <t>Sign</t>
+    <t>Shift</t>
   </si>
   <si>
-    <t>Shift</t>
+    <t>Sign</t>
   </si>
   <si>
     <t>UpperImm</t>
@@ -300,7 +300,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12.0"/>
       <color theme="1"/>
@@ -309,6 +309,11 @@
     <font>
       <sz val="12.0"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -341,7 +346,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -357,7 +362,10 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -647,16 +655,15 @@
       <c r="L2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="O2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
@@ -705,16 +712,15 @@
       <c r="L3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="M3" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="N3" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="N3" s="3">
-        <v>0.0</v>
       </c>
       <c r="O3" s="3">
         <v>0.0</v>
       </c>
-      <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
@@ -763,16 +769,15 @@
       <c r="L4" s="2">
         <v>1.0</v>
       </c>
-      <c r="M4" s="2">
+      <c r="M4" s="3">
         <v>1.0</v>
       </c>
-      <c r="N4" s="3">
-        <v>0.0</v>
+      <c r="N4" s="2">
+        <v>1.0</v>
       </c>
       <c r="O4" s="3">
         <v>0.0</v>
       </c>
-      <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
@@ -821,16 +826,15 @@
       <c r="L5" s="2">
         <v>1.0</v>
       </c>
-      <c r="M5" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="N5" s="3">
+      <c r="M5" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="N5" s="2">
         <v>0.0</v>
       </c>
       <c r="O5" s="3">
         <v>0.0</v>
       </c>
-      <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
       <c r="S5" s="2"/>
@@ -846,10 +850,10 @@
       <c r="A6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="5" t="s">
         <v>31</v>
       </c>
       <c r="D6" s="2">
@@ -879,16 +883,15 @@
       <c r="L6" s="2">
         <v>1.0</v>
       </c>
-      <c r="M6" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="N6" s="3">
+      <c r="M6" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="N6" s="2">
         <v>0.0</v>
       </c>
       <c r="O6" s="3">
         <v>0.0</v>
       </c>
-      <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
       <c r="S6" s="2"/>
@@ -937,16 +940,15 @@
       <c r="L7" s="2">
         <v>1.0</v>
       </c>
-      <c r="M7" s="2">
+      <c r="M7" s="3">
         <v>1.0</v>
       </c>
-      <c r="N7" s="3">
-        <v>0.0</v>
+      <c r="N7" s="2">
+        <v>1.0</v>
       </c>
       <c r="O7" s="3">
         <v>0.0</v>
       </c>
-      <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
       <c r="S7" s="2"/>
@@ -995,16 +997,15 @@
       <c r="L8" s="2">
         <v>1.0</v>
       </c>
-      <c r="M8" s="2">
+      <c r="M8" s="3">
         <v>1.0</v>
       </c>
-      <c r="N8" s="3">
-        <v>0.0</v>
+      <c r="N8" s="2">
+        <v>1.0</v>
       </c>
       <c r="O8" s="3">
         <v>0.0</v>
       </c>
-      <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
       <c r="S8" s="2"/>
@@ -1035,10 +1036,10 @@
       <c r="F9" s="2">
         <v>0.0</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="5">
         <v>0.0</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="5">
         <v>0.0</v>
       </c>
       <c r="I9" s="2" t="s">
@@ -1053,16 +1054,15 @@
       <c r="L9" s="2">
         <v>1.0</v>
       </c>
-      <c r="M9" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="N9" s="3">
-        <v>0.0</v>
+      <c r="M9" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="N9" s="5">
+        <v>1.0</v>
       </c>
       <c r="O9" s="3">
         <v>1.0</v>
       </c>
-      <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
       <c r="S9" s="2"/>
@@ -1093,10 +1093,10 @@
       <c r="F10" s="2">
         <v>0.0</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="5">
         <v>1.0</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="5">
         <v>1.0</v>
       </c>
       <c r="I10" s="3" t="s">
@@ -1115,12 +1115,11 @@
         <v>1.0</v>
       </c>
       <c r="N10" s="3">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="O10" s="3">
         <v>0.0</v>
       </c>
-      <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
       <c r="S10" s="2"/>
@@ -1169,16 +1168,15 @@
       <c r="L11" s="2">
         <v>1.0</v>
       </c>
-      <c r="M11" s="2">
+      <c r="M11" s="3">
         <v>1.0</v>
       </c>
-      <c r="N11" s="3">
-        <v>0.0</v>
+      <c r="N11" s="2">
+        <v>1.0</v>
       </c>
       <c r="O11" s="3">
         <v>0.0</v>
       </c>
-      <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
       <c r="S11" s="2"/>
@@ -1227,16 +1225,15 @@
       <c r="L12" s="2">
         <v>1.0</v>
       </c>
-      <c r="M12" s="2">
+      <c r="M12" s="3">
         <v>1.0</v>
       </c>
-      <c r="N12" s="3">
-        <v>0.0</v>
+      <c r="N12" s="2">
+        <v>1.0</v>
       </c>
       <c r="O12" s="3">
         <v>0.0</v>
       </c>
-      <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
       <c r="S12" s="2"/>
@@ -1285,16 +1282,15 @@
       <c r="L13" s="2">
         <v>1.0</v>
       </c>
-      <c r="M13" s="2">
+      <c r="M13" s="3">
         <v>1.0</v>
       </c>
-      <c r="N13" s="3">
-        <v>0.0</v>
+      <c r="N13" s="2">
+        <v>1.0</v>
       </c>
       <c r="O13" s="3">
         <v>0.0</v>
       </c>
-      <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
       <c r="S13" s="2"/>
@@ -1343,16 +1339,15 @@
       <c r="L14" s="2">
         <v>1.0</v>
       </c>
-      <c r="M14" s="2">
+      <c r="M14" s="3">
         <v>1.0</v>
       </c>
-      <c r="N14" s="3">
-        <v>0.0</v>
+      <c r="N14" s="2">
+        <v>1.0</v>
       </c>
       <c r="O14" s="3">
         <v>0.0</v>
       </c>
-      <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
       <c r="S14" s="2"/>
@@ -1401,16 +1396,15 @@
       <c r="L15" s="2">
         <v>1.0</v>
       </c>
-      <c r="M15" s="2">
+      <c r="M15" s="3">
         <v>1.0</v>
       </c>
-      <c r="N15" s="3">
-        <v>0.0</v>
+      <c r="N15" s="2">
+        <v>1.0</v>
       </c>
       <c r="O15" s="3">
         <v>0.0</v>
       </c>
-      <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
       <c r="S15" s="2"/>
@@ -1459,16 +1453,15 @@
       <c r="L16" s="2">
         <v>1.0</v>
       </c>
-      <c r="M16" s="2">
+      <c r="M16" s="3">
         <v>1.0</v>
       </c>
-      <c r="N16" s="3">
-        <v>0.0</v>
+      <c r="N16" s="2">
+        <v>1.0</v>
       </c>
       <c r="O16" s="3">
         <v>0.0</v>
       </c>
-      <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
       <c r="S16" s="2"/>
@@ -1517,16 +1510,15 @@
       <c r="L17" s="2">
         <v>1.0</v>
       </c>
-      <c r="M17" s="2">
+      <c r="M17" s="3">
         <v>1.0</v>
       </c>
-      <c r="N17" s="3">
-        <v>0.0</v>
+      <c r="N17" s="2">
+        <v>1.0</v>
       </c>
       <c r="O17" s="3">
         <v>0.0</v>
       </c>
-      <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
       <c r="S17" s="2"/>
@@ -1563,7 +1555,7 @@
       <c r="H18" s="2">
         <v>0.0</v>
       </c>
-      <c r="I18" s="5" t="s">
+      <c r="I18" s="6" t="s">
         <v>54</v>
       </c>
       <c r="J18" s="2">
@@ -1575,16 +1567,15 @@
       <c r="L18" s="2">
         <v>1.0</v>
       </c>
-      <c r="M18" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="N18" s="3">
+      <c r="M18" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="N18" s="2">
         <v>0.0</v>
       </c>
       <c r="O18" s="3">
         <v>0.0</v>
       </c>
-      <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
       <c r="S18" s="2"/>
@@ -1603,7 +1594,7 @@
       <c r="B19" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="5" t="s">
         <v>60</v>
       </c>
       <c r="D19" s="2">
@@ -1621,7 +1612,7 @@
       <c r="H19" s="2">
         <v>0.0</v>
       </c>
-      <c r="I19" s="5" t="s">
+      <c r="I19" s="6" t="s">
         <v>54</v>
       </c>
       <c r="J19" s="2">
@@ -1633,16 +1624,15 @@
       <c r="L19" s="2">
         <v>1.0</v>
       </c>
-      <c r="M19" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="N19" s="3">
+      <c r="M19" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="N19" s="2">
         <v>0.0</v>
       </c>
       <c r="O19" s="3">
         <v>0.0</v>
       </c>
-      <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
       <c r="S19" s="2"/>
@@ -1691,16 +1681,15 @@
       <c r="L20" s="2">
         <v>1.0</v>
       </c>
-      <c r="M20" s="2">
+      <c r="M20" s="3">
         <v>1.0</v>
       </c>
-      <c r="N20" s="3">
-        <v>0.0</v>
+      <c r="N20" s="2">
+        <v>1.0</v>
       </c>
       <c r="O20" s="3">
         <v>0.0</v>
       </c>
-      <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
       <c r="R20" s="2"/>
       <c r="S20" s="2"/>
@@ -1749,16 +1738,15 @@
       <c r="L21" s="2">
         <v>1.0</v>
       </c>
-      <c r="M21" s="2">
+      <c r="M21" s="3">
         <v>1.0</v>
       </c>
-      <c r="N21" s="3">
-        <v>0.0</v>
+      <c r="N21" s="2">
+        <v>1.0</v>
       </c>
       <c r="O21" s="3">
         <v>0.0</v>
       </c>
-      <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
       <c r="R21" s="2"/>
       <c r="S21" s="2"/>
@@ -1807,16 +1795,15 @@
       <c r="L22" s="2">
         <v>1.0</v>
       </c>
-      <c r="M22" s="2">
+      <c r="M22" s="3">
         <v>1.0</v>
       </c>
-      <c r="N22" s="3">
-        <v>0.0</v>
+      <c r="N22" s="2">
+        <v>1.0</v>
       </c>
       <c r="O22" s="3">
         <v>0.0</v>
       </c>
-      <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
       <c r="S22" s="2"/>
@@ -1853,7 +1840,7 @@
       <c r="H23" s="2">
         <v>0.0</v>
       </c>
-      <c r="I23" s="5" t="s">
+      <c r="I23" s="6" t="s">
         <v>62</v>
       </c>
       <c r="J23" s="2">
@@ -1865,16 +1852,15 @@
       <c r="L23" s="2">
         <v>1.0</v>
       </c>
-      <c r="M23" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="N23" s="3">
+      <c r="M23" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="N23" s="2">
         <v>1.0</v>
       </c>
       <c r="O23" s="3">
         <v>0.0</v>
       </c>
-      <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
       <c r="S23" s="2"/>
@@ -1911,7 +1897,7 @@
       <c r="H24" s="2">
         <v>0.0</v>
       </c>
-      <c r="I24" s="5" t="s">
+      <c r="I24" s="6" t="s">
         <v>64</v>
       </c>
       <c r="J24" s="2">
@@ -1923,16 +1909,15 @@
       <c r="L24" s="2">
         <v>1.0</v>
       </c>
-      <c r="M24" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="N24" s="3">
+      <c r="M24" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="N24" s="2">
         <v>1.0</v>
       </c>
       <c r="O24" s="3">
         <v>0.0</v>
       </c>
-      <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
       <c r="S24" s="2"/>
@@ -1969,7 +1954,7 @@
       <c r="H25" s="2">
         <v>0.0</v>
       </c>
-      <c r="I25" s="5" t="s">
+      <c r="I25" s="6" t="s">
         <v>66</v>
       </c>
       <c r="J25" s="2">
@@ -1981,16 +1966,15 @@
       <c r="L25" s="2">
         <v>1.0</v>
       </c>
-      <c r="M25" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="N25" s="3">
+      <c r="M25" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="N25" s="2">
         <v>1.0</v>
       </c>
       <c r="O25" s="3">
         <v>0.0</v>
       </c>
-      <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
       <c r="S25" s="2"/>
@@ -2039,16 +2023,15 @@
       <c r="L26" s="2">
         <v>0.0</v>
       </c>
-      <c r="M26" s="2">
+      <c r="M26" s="3">
         <v>1.0</v>
       </c>
-      <c r="N26" s="3">
-        <v>0.0</v>
+      <c r="N26" s="2">
+        <v>1.0</v>
       </c>
       <c r="O26" s="3">
         <v>0.0</v>
       </c>
-      <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
       <c r="R26" s="2"/>
       <c r="S26" s="2"/>
@@ -2097,16 +2080,15 @@
       <c r="L27" s="2">
         <v>1.0</v>
       </c>
-      <c r="M27" s="2">
+      <c r="M27" s="3">
         <v>1.0</v>
       </c>
-      <c r="N27" s="3">
-        <v>0.0</v>
+      <c r="N27" s="2">
+        <v>1.0</v>
       </c>
       <c r="O27" s="3">
         <v>0.0</v>
       </c>
-      <c r="P27" s="2"/>
       <c r="Q27" s="2"/>
       <c r="R27" s="2"/>
       <c r="S27" s="2"/>
@@ -2125,7 +2107,7 @@
       <c r="B28" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="5" t="s">
         <v>38</v>
       </c>
       <c r="D28" s="2">
@@ -2143,7 +2125,7 @@
       <c r="H28" s="2">
         <v>0.0</v>
       </c>
-      <c r="I28" s="5" t="s">
+      <c r="I28" s="6" t="s">
         <v>76</v>
       </c>
       <c r="J28" s="2">
@@ -2155,16 +2137,15 @@
       <c r="L28" s="2">
         <v>1.0</v>
       </c>
-      <c r="M28" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="N28" s="3">
+      <c r="M28" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="N28" s="2">
         <v>0.0</v>
       </c>
       <c r="O28" s="3">
         <v>0.0</v>
       </c>
-      <c r="P28" s="2"/>
       <c r="Q28" s="2"/>
       <c r="R28" s="2"/>
       <c r="S28" s="2"/>
@@ -2209,16 +2190,15 @@
       <c r="L29" s="2">
         <v>0.0</v>
       </c>
-      <c r="M29" s="2">
+      <c r="M29" s="3">
         <v>1.0</v>
       </c>
-      <c r="N29" s="3">
-        <v>0.0</v>
+      <c r="N29" s="2">
+        <v>1.0</v>
       </c>
       <c r="O29" s="3">
         <v>0.0</v>
       </c>
-      <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
       <c r="R29" s="2"/>
       <c r="S29" s="2"/>
@@ -2263,16 +2243,15 @@
       <c r="L30" s="2">
         <v>0.0</v>
       </c>
-      <c r="M30" s="2">
+      <c r="M30" s="3">
         <v>1.0</v>
       </c>
-      <c r="N30" s="3">
-        <v>0.0</v>
+      <c r="N30" s="2">
+        <v>1.0</v>
       </c>
       <c r="O30" s="3">
         <v>0.0</v>
       </c>
-      <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
       <c r="R30" s="2"/>
       <c r="S30" s="2"/>
@@ -2317,16 +2296,15 @@
       <c r="L31" s="2">
         <v>0.0</v>
       </c>
-      <c r="M31" s="2">
+      <c r="M31" s="3">
         <v>1.0</v>
       </c>
-      <c r="N31" s="3">
-        <v>0.0</v>
+      <c r="N31" s="2">
+        <v>1.0</v>
       </c>
       <c r="O31" s="3">
         <v>0.0</v>
       </c>
-      <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
       <c r="S31" s="2"/>
@@ -2371,16 +2349,15 @@
       <c r="L32" s="2">
         <v>1.0</v>
       </c>
-      <c r="M32" s="2">
+      <c r="M32" s="3">
         <v>1.0</v>
       </c>
-      <c r="N32" s="3">
+      <c r="N32" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="O32" s="5">
         <v>0.0</v>
       </c>
-      <c r="O32" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
       <c r="S32" s="2"/>
@@ -2425,16 +2402,15 @@
       <c r="L33" s="2">
         <v>0.0</v>
       </c>
-      <c r="M33" s="2">
+      <c r="M33" s="3">
         <v>1.0</v>
       </c>
-      <c r="N33" s="3">
+      <c r="N33" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="O33" s="5">
         <v>0.0</v>
       </c>
-      <c r="O33" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="P33" s="2"/>
       <c r="Q33" s="2"/>
       <c r="R33" s="2"/>
       <c r="S33" s="2"/>

</xml_diff>

<commit_message>
fixed buggs errors and starting testing.
</commit_message>
<xml_diff>
--- a/Project_B/control_signals_template.xlsx
+++ b/Project_B/control_signals_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\cpre381\cpre-381-projects\Project_B\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DBC346A-5832-4982-8DE6-37F35508498F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90554F0A-C58D-4B50-837C-CEA1D480AF26}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="87">
   <si>
     <t>Instruction</t>
   </si>
@@ -310,6 +310,9 @@
   </si>
   <si>
     <t>"11010"</t>
+  </si>
+  <si>
+    <t>"100100"</t>
   </si>
 </sst>
 </file>
@@ -629,7 +632,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I30" sqref="I30"/>
+      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1"/>
@@ -970,7 +973,7 @@
         <v>26</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>27</v>
+        <v>86</v>
       </c>
       <c r="D7" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
bug on fib example going to update all the test framework files
</commit_message>
<xml_diff>
--- a/Project_B/control_signals_template.xlsx
+++ b/Project_B/control_signals_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\cpre381\cpre-381-projects\Project_B\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90554F0A-C58D-4B50-837C-CEA1D480AF26}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4B7D90-CE47-4ADC-B3FB-C14648BB9C3E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -632,7 +632,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomRight" activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1"/>

</xml_diff>